<commit_message>
CN_05_12_CO con corrección de estilo y revisión final editor
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado05/guion12/EsqueletoGuion_CN_05_12_CO.xlsx
+++ b/fuentes/contenidos/grado05/guion12/EsqueletoGuion_CN_05_12_CO.xlsx
@@ -19,7 +19,7 @@
     <sheet name="CUADERNO DE ESTUDIO" sheetId="16" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'CUADERNO DE ESTUDIO'!$A$1:$I$82</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'CUADERNO DE ESTUDIO'!$A$1:$I$79</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'RECURSOS NUEVOS'!$A$1:$C$23</definedName>
   </definedNames>
   <calcPr calcId="124519" concurrentCalc="0"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="72">
   <si>
     <t>FICHA</t>
   </si>
@@ -133,9 +133,6 @@
     <t>Evaluación</t>
   </si>
   <si>
-    <t>Fin de tema</t>
-  </si>
-  <si>
     <t>CN_05_12_CO</t>
   </si>
   <si>
@@ -169,9 +166,6 @@
     <t>Utilización de las máquinas eléctricas en diferentes actividades humanas</t>
   </si>
   <si>
-    <t>¿Cómo usan la electricidad las máquinas eléctricas?</t>
-  </si>
-  <si>
     <t xml:space="preserve">La producción de calor a partir de la electricidad </t>
   </si>
   <si>
@@ -187,21 +181,12 @@
     <t>Otras aplicaciones de la electricidad</t>
   </si>
   <si>
-    <t>PENDIENTE</t>
-  </si>
-  <si>
     <t>Máquinas eléctricas y el tipo de energía que generan</t>
   </si>
   <si>
     <t>Los electrodomésticos</t>
   </si>
   <si>
-    <t>Peligros por el mal uso de las máquinas eléctricas</t>
-  </si>
-  <si>
-    <t>Algunas medidas relacionadas con el manejo seguro  de la electricidad</t>
-  </si>
-  <si>
     <t>El uso de la electricidad en las máquinas eléctricas</t>
   </si>
   <si>
@@ -211,9 +196,6 @@
     <t>Los generadores magneto-mecánicos</t>
   </si>
   <si>
-    <t>Las hidroeléctricas</t>
-  </si>
-  <si>
     <t>Las turbinas eólicas</t>
   </si>
   <si>
@@ -247,17 +229,35 @@
     <t>Nikola Tesla y la conducción de la electricidad sin cables</t>
   </si>
   <si>
-    <t>El tren eléctrico sin ruedas del Japón</t>
-  </si>
-  <si>
-    <t>¿Generan realmente las hidroeléctricas energía limpia?</t>
+    <t>¿Cómo las máquinas eléctricas usan la electricidad?</t>
+  </si>
+  <si>
+    <t>Peligros de hacer mal uso de las máquinas eléctricas</t>
+  </si>
+  <si>
+    <t>¿Qué es el tren Maglev?</t>
+  </si>
+  <si>
+    <t>¿Generan realmente energía limpia las hidroeléctricas?</t>
+  </si>
+  <si>
+    <t>Evaluación sobre las máquinas eléctricas</t>
+  </si>
+  <si>
+    <t>Algunas medidas relacionadas con el manejo seguro de la electricidad</t>
+  </si>
+  <si>
+    <t>Fin de unidad</t>
+  </si>
+  <si>
+    <t>Las centrales hidroeléctricas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -337,14 +337,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color theme="4" tint="-0.249977111117893"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -375,6 +369,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -801,7 +801,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -899,8 +899,10 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="401">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -1584,7 +1586,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1598,7 +1600,7 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1606,7 +1608,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1614,7 +1616,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1622,7 +1624,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1731,7 +1733,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23:C24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1751,10 +1755,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="49" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="52" t="s">
         <v>21</v>
       </c>
       <c r="C2">
@@ -1762,8 +1766,8 @@
       </c>
     </row>
     <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>41</v>
+      <c r="A3" s="51" t="s">
+        <v>40</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>20</v>
@@ -1773,8 +1777,8 @@
       </c>
     </row>
     <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>42</v>
+      <c r="A4" s="51" t="s">
+        <v>41</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>20</v>
@@ -1784,8 +1788,8 @@
       </c>
     </row>
     <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>43</v>
+      <c r="A5" s="51" t="s">
+        <v>42</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>20</v>
@@ -1795,8 +1799,8 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>48</v>
+      <c r="A6" s="51" t="s">
+        <v>46</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>20</v>
@@ -1806,8 +1810,10 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="50"/>
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="52" t="s">
         <v>21</v>
       </c>
       <c r="C7">
@@ -1815,8 +1821,8 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>51</v>
+      <c r="A8" s="51" t="s">
+        <v>48</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>20</v>
@@ -1826,8 +1832,8 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>52</v>
+      <c r="A9" s="51" t="s">
+        <v>49</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>20</v>
@@ -1837,10 +1843,10 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="50" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" s="4" t="s">
+      <c r="A10" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="52" t="s">
         <v>21</v>
       </c>
       <c r="C10">
@@ -1848,8 +1854,8 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>55</v>
+      <c r="A11" s="51" t="s">
+        <v>50</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>20</v>
@@ -1859,8 +1865,8 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>60</v>
+      <c r="A12" s="51" t="s">
+        <v>54</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>20</v>
@@ -1870,8 +1876,8 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>63</v>
+      <c r="A13" s="51" t="s">
+        <v>57</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>20</v>
@@ -1881,8 +1887,8 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>65</v>
+      <c r="A14" s="51" t="s">
+        <v>59</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>20</v>
@@ -1892,8 +1898,8 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>66</v>
+      <c r="A15" s="51" t="s">
+        <v>60</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>20</v>
@@ -1902,11 +1908,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="B16" s="4" t="s">
+    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="52" t="s">
         <v>21</v>
       </c>
       <c r="C16">
@@ -1914,8 +1920,8 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>68</v>
+      <c r="A17" s="51" t="s">
+        <v>62</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>20</v>
@@ -1925,8 +1931,8 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>69</v>
+      <c r="A18" s="51" t="s">
+        <v>63</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>20</v>
@@ -1936,8 +1942,8 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>70</v>
+      <c r="A19" s="51" t="s">
+        <v>66</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>20</v>
@@ -1947,18 +1953,18 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>71</v>
+      <c r="A20" s="49" t="s">
+        <v>67</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C20">
         <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="51" t="s">
         <v>22</v>
       </c>
       <c r="B21" s="4" t="s">
@@ -1969,11 +1975,11 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="50" t="s">
-        <v>34</v>
+      <c r="A22" s="51" t="s">
+        <v>68</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C22">
         <v>21</v>
@@ -2004,7 +2010,9 @@
   </sheetPr>
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2028,8 +2036,8 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="50" t="s">
-        <v>39</v>
+      <c r="B2" s="49" t="s">
+        <v>38</v>
       </c>
       <c r="C2" t="s">
         <v>20</v>
@@ -2040,7 +2048,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
@@ -2051,7 +2059,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
@@ -2062,7 +2070,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
         <v>20</v>
@@ -2073,7 +2081,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s">
         <v>20</v>
@@ -2083,7 +2091,9 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="50"/>
+      <c r="B7" s="49" t="s">
+        <v>64</v>
+      </c>
       <c r="C7" t="s">
         <v>20</v>
       </c>
@@ -2093,7 +2103,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
@@ -2104,7 +2114,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C9" t="s">
         <v>20</v>
@@ -2114,8 +2124,8 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="50" t="s">
-        <v>54</v>
+      <c r="B10" s="49" t="s">
+        <v>69</v>
       </c>
       <c r="C10" t="s">
         <v>20</v>
@@ -2126,7 +2136,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C11" t="s">
         <v>20</v>
@@ -2137,7 +2147,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C12" t="s">
         <v>20</v>
@@ -2148,7 +2158,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C13" t="s">
         <v>20</v>
@@ -2159,7 +2169,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C14" t="s">
         <v>20</v>
@@ -2170,7 +2180,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C15" t="s">
         <v>20</v>
@@ -2180,8 +2190,8 @@
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="50" t="s">
-        <v>67</v>
+      <c r="B16" s="49" t="s">
+        <v>61</v>
       </c>
       <c r="C16" t="s">
         <v>20</v>
@@ -2192,7 +2202,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C17" t="s">
         <v>20</v>
@@ -2203,7 +2213,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C18" t="s">
         <v>20</v>
@@ -2214,7 +2224,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C19" t="s">
         <v>20</v>
@@ -2225,7 +2235,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C20" t="s">
         <v>20</v>
@@ -2246,8 +2256,8 @@
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="50" t="s">
-        <v>34</v>
+      <c r="B22" s="49" t="s">
+        <v>68</v>
       </c>
       <c r="C22" t="s">
         <v>20</v>
@@ -2276,11 +2286,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X83"/>
+  <dimension ref="A1:X80"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F60" sqref="F60"/>
+      <selection pane="bottomLeft" activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2292,7 +2302,7 @@
     <col min="5" max="5" width="17.85546875" style="3" customWidth="1"/>
     <col min="6" max="6" width="21.7109375" style="3" customWidth="1"/>
     <col min="7" max="7" width="17.85546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="52.140625" customWidth="1"/>
+    <col min="8" max="8" width="74.7109375" customWidth="1"/>
     <col min="9" max="9" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2327,10 +2337,10 @@
     </row>
     <row r="2" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>23</v>
@@ -2342,13 +2352,13 @@
     </row>
     <row r="3" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>37</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>38</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>23</v>
@@ -2358,14 +2368,14 @@
     </row>
     <row r="4" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="24"/>
       <c r="D4" s="29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E4" s="29" t="s">
         <v>27</v>
@@ -2373,7 +2383,7 @@
       <c r="F4" s="29"/>
       <c r="G4" s="29"/>
       <c r="H4" s="24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I4" s="24" t="s">
         <v>20</v>
@@ -2381,13 +2391,13 @@
     </row>
     <row r="5" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E5" s="26" t="s">
         <v>23</v>
@@ -2397,14 +2407,14 @@
     </row>
     <row r="6" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E6" s="26" t="s">
         <v>29</v>
@@ -2415,14 +2425,14 @@
     </row>
     <row r="7" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" s="20"/>
       <c r="D7" s="26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E7" s="26" t="s">
         <v>24</v>
@@ -2436,14 +2446,14 @@
     </row>
     <row r="8" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8" s="35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" s="31"/>
       <c r="D8" s="32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E8" s="32" t="s">
         <v>26</v>
@@ -2451,7 +2461,7 @@
       <c r="F8" s="33"/>
       <c r="G8" s="33"/>
       <c r="H8" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I8" s="31" t="s">
         <v>20</v>
@@ -2461,14 +2471,14 @@
     </row>
     <row r="9" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="20"/>
       <c r="D9" s="26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E9" s="26" t="s">
         <v>23</v>
@@ -2482,14 +2492,14 @@
     </row>
     <row r="10" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="20"/>
       <c r="D10" s="26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E10" s="26" t="s">
         <v>24</v>
@@ -2503,14 +2513,14 @@
     </row>
     <row r="11" spans="1:11" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" s="20"/>
       <c r="D11" s="26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E11" s="26" t="s">
         <v>25</v>
@@ -2522,14 +2532,14 @@
     </row>
     <row r="12" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" s="20"/>
       <c r="D12" s="26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E12" s="26" t="s">
         <v>23</v>
@@ -2541,14 +2551,14 @@
     </row>
     <row r="13" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13" s="35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" s="31"/>
       <c r="D13" s="32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E13" s="32" t="s">
         <v>26</v>
@@ -2556,7 +2566,7 @@
       <c r="F13" s="33"/>
       <c r="G13" s="33"/>
       <c r="H13" s="34" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I13" s="34" t="s">
         <v>20</v>
@@ -2564,14 +2574,14 @@
     </row>
     <row r="14" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14" s="35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C14" s="31"/>
       <c r="D14" s="32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E14" s="32" t="s">
         <v>26</v>
@@ -2579,7 +2589,7 @@
       <c r="F14" s="36"/>
       <c r="G14" s="33"/>
       <c r="H14" s="34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I14" s="34" t="s">
         <v>20</v>
@@ -2587,10 +2597,10 @@
     </row>
     <row r="15" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C15" s="20" t="s">
         <v>23</v>
@@ -2604,14 +2614,14 @@
     </row>
     <row r="16" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C16" s="20"/>
       <c r="D16" s="21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E16" s="21" t="s">
         <v>23</v>
@@ -2623,14 +2633,14 @@
     </row>
     <row r="17" spans="1:24" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C17" s="20"/>
       <c r="D17" s="21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E17" s="21" t="s">
         <v>29</v>
@@ -2642,14 +2652,14 @@
     </row>
     <row r="18" spans="1:24" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C18" s="20"/>
       <c r="D18" s="21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E18" s="21" t="s">
         <v>23</v>
@@ -2661,14 +2671,14 @@
     </row>
     <row r="19" spans="1:24" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C19" s="20"/>
       <c r="D19" s="21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E19" s="21" t="s">
         <v>24</v>
@@ -2680,14 +2690,14 @@
     </row>
     <row r="20" spans="1:24" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C20" s="20"/>
       <c r="D20" s="21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E20" s="21" t="s">
         <v>23</v>
@@ -2699,14 +2709,14 @@
     </row>
     <row r="21" spans="1:24" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C21" s="20"/>
       <c r="D21" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E21" s="26" t="s">
         <v>23</v>
@@ -2718,14 +2728,14 @@
     </row>
     <row r="22" spans="1:24" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C22" s="20"/>
       <c r="D22" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E22" s="26" t="s">
         <v>24</v>
@@ -2737,14 +2747,14 @@
     </row>
     <row r="23" spans="1:24" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C23" s="20"/>
       <c r="D23" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E23" s="26" t="s">
         <v>23</v>
@@ -2756,14 +2766,14 @@
     </row>
     <row r="24" spans="1:24" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C24" s="20"/>
       <c r="D24" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E24" s="26" t="s">
         <v>28</v>
@@ -2775,14 +2785,14 @@
     </row>
     <row r="25" spans="1:24" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C25" s="20"/>
       <c r="D25" s="37" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E25" s="9" t="s">
         <v>23</v>
@@ -2794,14 +2804,14 @@
     </row>
     <row r="26" spans="1:24" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C26" s="20"/>
       <c r="D26" s="37" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E26" s="9" t="s">
         <v>29</v>
@@ -2813,14 +2823,14 @@
     </row>
     <row r="27" spans="1:24" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C27" s="20"/>
       <c r="D27" s="37" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E27" s="9" t="s">
         <v>23</v>
@@ -2832,14 +2842,14 @@
     </row>
     <row r="28" spans="1:24" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C28" s="20"/>
       <c r="D28" s="37" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E28" s="9" t="s">
         <v>24</v>
@@ -2851,14 +2861,14 @@
     </row>
     <row r="29" spans="1:24" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C29" s="20"/>
       <c r="D29" s="37" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E29" s="9" t="s">
         <v>23</v>
@@ -2868,16 +2878,16 @@
       <c r="H29" s="20"/>
       <c r="I29" s="21"/>
     </row>
-    <row r="30" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B30" s="31" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C30" s="31"/>
       <c r="D30" s="38" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E30" s="39" t="s">
         <v>26</v>
@@ -2885,7 +2895,7 @@
       <c r="F30" s="33"/>
       <c r="G30" s="33"/>
       <c r="H30" s="40" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I30" s="39" t="s">
         <v>20</v>
@@ -2893,14 +2903,14 @@
     </row>
     <row r="31" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C31" s="18"/>
       <c r="D31" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E31" s="19" t="s">
         <v>23</v>
@@ -2927,14 +2937,14 @@
     </row>
     <row r="32" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C32" s="18"/>
       <c r="D32" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E32" s="19" t="s">
         <v>24</v>
@@ -2961,14 +2971,14 @@
     </row>
     <row r="33" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33" s="20" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C33" s="18"/>
       <c r="D33" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E33" s="19" t="s">
         <v>23</v>
@@ -2995,14 +3005,14 @@
     </row>
     <row r="34" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34" s="20" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C34" s="18"/>
       <c r="D34" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E34" s="19" t="s">
         <v>24</v>
@@ -3029,14 +3039,14 @@
     </row>
     <row r="35" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35" s="20" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C35" s="18"/>
       <c r="D35" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E35" s="19" t="s">
         <v>23</v>
@@ -3063,14 +3073,14 @@
     </row>
     <row r="36" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B36" s="20" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C36" s="18"/>
       <c r="D36" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E36" s="19" t="s">
         <v>24</v>
@@ -3097,14 +3107,14 @@
     </row>
     <row r="37" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C37" s="18"/>
       <c r="D37" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E37" s="19" t="s">
         <v>23</v>
@@ -3131,14 +3141,14 @@
     </row>
     <row r="38" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B38" s="20" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C38" s="18"/>
       <c r="D38" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E38" s="19" t="s">
         <v>24</v>
@@ -3165,21 +3175,23 @@
     </row>
     <row r="39" spans="1:24" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B39" s="44" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C39" s="43"/>
       <c r="D39" s="28" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E39" s="29" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="F39" s="28"/>
       <c r="G39" s="28"/>
-      <c r="H39" s="43"/>
+      <c r="H39" s="43" t="s">
+        <v>64</v>
+      </c>
       <c r="I39" s="43" t="s">
         <v>20</v>
       </c>
@@ -3199,24 +3211,24 @@
       <c r="W39" s="43"/>
       <c r="X39" s="43"/>
     </row>
-    <row r="40" spans="1:24" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B40" s="31" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C40" s="41"/>
       <c r="D40" s="42" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E40" s="42" t="s">
         <v>26</v>
       </c>
       <c r="F40" s="42"/>
       <c r="G40" s="42"/>
-      <c r="H40" s="49" t="s">
-        <v>51</v>
+      <c r="H40" s="50" t="s">
+        <v>48</v>
       </c>
       <c r="I40" s="41" t="s">
         <v>20</v>
@@ -3237,24 +3249,24 @@
       <c r="W40" s="18"/>
       <c r="X40" s="18"/>
     </row>
-    <row r="41" spans="1:24" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B41" s="31" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C41" s="41"/>
       <c r="D41" s="42" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E41" s="42" t="s">
         <v>26</v>
       </c>
       <c r="F41" s="42"/>
       <c r="G41" s="42"/>
-      <c r="H41" s="49" t="s">
-        <v>52</v>
+      <c r="H41" s="50" t="s">
+        <v>49</v>
       </c>
       <c r="I41" s="41" t="s">
         <v>20</v>
@@ -3277,14 +3289,14 @@
     </row>
     <row r="42" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B42" s="20" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C42" s="17"/>
       <c r="D42" s="27" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="E42" s="27" t="s">
         <v>23</v>
@@ -3311,14 +3323,14 @@
     </row>
     <row r="43" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B43" s="20" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C43" s="17"/>
       <c r="D43" s="27" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="E43" s="27" t="s">
         <v>24</v>
@@ -3345,14 +3357,14 @@
     </row>
     <row r="44" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B44" s="20" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C44" s="17"/>
       <c r="D44" s="27" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="E44" s="27" t="s">
         <v>23</v>
@@ -3379,14 +3391,14 @@
     </row>
     <row r="45" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B45" s="44" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C45" s="45"/>
       <c r="D45" s="46" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="E45" s="46" t="s">
         <v>27</v>
@@ -3394,7 +3406,7 @@
       <c r="F45" s="46"/>
       <c r="G45" s="46"/>
       <c r="H45" s="45" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="I45" s="43" t="s">
         <v>20</v>
@@ -3417,160 +3429,156 @@
     </row>
     <row r="46" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B46" s="20" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C46" s="17"/>
-      <c r="D46" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="E46" s="27"/>
-      <c r="F46" s="27"/>
-      <c r="G46" s="27"/>
-      <c r="H46" s="17"/>
-      <c r="I46" s="19"/>
-      <c r="J46" s="18"/>
-      <c r="K46" s="18"/>
-      <c r="L46" s="18"/>
-      <c r="M46" s="18"/>
-      <c r="N46" s="18"/>
-      <c r="O46" s="18"/>
-      <c r="P46" s="18"/>
-      <c r="Q46" s="18"/>
-      <c r="R46" s="18"/>
-      <c r="S46" s="18"/>
-      <c r="T46" s="18"/>
-      <c r="U46" s="18"/>
-      <c r="V46" s="18"/>
-      <c r="W46" s="18"/>
-      <c r="X46" s="18"/>
+      <c r="D46" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="E46" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F46" s="26"/>
+      <c r="G46" s="26"/>
+      <c r="H46" s="16"/>
+      <c r="I46" s="17"/>
+      <c r="J46" s="17"/>
+      <c r="K46" s="16"/>
+      <c r="L46" s="16"/>
     </row>
     <row r="47" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B47" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="C47" s="17"/>
-      <c r="D47" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="E47" s="27"/>
-      <c r="F47" s="27"/>
-      <c r="G47" s="27"/>
-      <c r="H47" s="17"/>
-      <c r="I47" s="17"/>
+      <c r="A47" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B47" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="C47" s="35"/>
+      <c r="D47" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="E47" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="F47" s="32"/>
+      <c r="G47" s="32"/>
+      <c r="H47" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="I47" s="35" t="s">
+        <v>20</v>
+      </c>
       <c r="J47" s="17"/>
       <c r="K47" s="16"/>
       <c r="L47" s="16"/>
     </row>
     <row r="48" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B48" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="C48" s="17"/>
-      <c r="D48" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="E48" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C48" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F48" s="26"/>
-      <c r="G48" s="26"/>
-      <c r="H48" s="16"/>
-      <c r="I48" s="17"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="8"/>
       <c r="J48" s="17"/>
       <c r="K48" s="16"/>
       <c r="L48" s="16"/>
     </row>
     <row r="49" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="B49" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="C49" s="35"/>
-      <c r="D49" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="E49" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="F49" s="32"/>
-      <c r="G49" s="32"/>
-      <c r="H49" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="I49" s="35" t="s">
-        <v>20</v>
-      </c>
+      <c r="A49" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C49" s="8"/>
+      <c r="D49" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E49" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="8"/>
       <c r="J49" s="17"/>
       <c r="K49" s="16"/>
       <c r="L49" s="16"/>
     </row>
-    <row r="50" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C50" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C50" s="8"/>
+      <c r="D50" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G50" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9"/>
       <c r="H50" s="8"/>
       <c r="I50" s="8"/>
       <c r="J50" s="17"/>
       <c r="K50" s="16"/>
       <c r="L50" s="16"/>
     </row>
-    <row r="51" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C51" s="8"/>
       <c r="D51" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E51" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F51" s="9"/>
-      <c r="G51" s="9"/>
+        <v>52</v>
+      </c>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G51" s="9" t="s">
+        <v>24</v>
+      </c>
       <c r="H51" s="8"/>
       <c r="I51" s="8"/>
       <c r="J51" s="17"/>
       <c r="K51" s="16"/>
       <c r="L51" s="16"/>
     </row>
-    <row r="52" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C52" s="8"/>
       <c r="D52" s="9" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E52" s="9"/>
       <c r="F52" s="9" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="G52" s="9" t="s">
         <v>23</v>
@@ -3583,21 +3591,21 @@
     </row>
     <row r="53" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C53" s="8"/>
       <c r="D53" s="9" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E53" s="9"/>
-      <c r="F53" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="G53" s="9" t="s">
-        <v>24</v>
+      <c r="F53" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="G53" s="26" t="s">
+        <v>23</v>
       </c>
       <c r="H53" s="8"/>
       <c r="I53" s="8"/>
@@ -3607,21 +3615,21 @@
     </row>
     <row r="54" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C54" s="8"/>
       <c r="D54" s="9" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E54" s="9"/>
-      <c r="F54" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="G54" s="9" t="s">
-        <v>23</v>
+      <c r="F54" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="G54" s="26" t="s">
+        <v>24</v>
       </c>
       <c r="H54" s="8"/>
       <c r="I54" s="8"/>
@@ -3631,18 +3639,18 @@
     </row>
     <row r="55" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C55" s="8"/>
       <c r="D55" s="9" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E55" s="9"/>
       <c r="F55" s="26" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="G55" s="26" t="s">
         <v>23</v>
@@ -3655,62 +3663,58 @@
     </row>
     <row r="56" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C56" s="8"/>
-      <c r="D56" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E56" s="9"/>
-      <c r="F56" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="G56" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="H56" s="8"/>
-      <c r="I56" s="8"/>
+        <v>51</v>
+      </c>
+      <c r="C56" s="17"/>
+      <c r="D56" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="E56" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F56" s="21"/>
+      <c r="G56" s="21"/>
+      <c r="H56" s="20"/>
+      <c r="I56" s="20"/>
       <c r="J56" s="17"/>
       <c r="K56" s="16"/>
       <c r="L56" s="16"/>
     </row>
     <row r="57" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C57" s="8"/>
-      <c r="D57" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E57" s="9"/>
-      <c r="F57" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="G57" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="H57" s="8"/>
-      <c r="I57" s="8"/>
+        <v>51</v>
+      </c>
+      <c r="C57" s="17"/>
+      <c r="D57" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="E57" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="F57" s="21"/>
+      <c r="G57" s="21"/>
+      <c r="H57" s="20"/>
+      <c r="I57" s="20"/>
       <c r="J57" s="17"/>
       <c r="K57" s="16"/>
       <c r="L57" s="16"/>
     </row>
     <row r="58" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C58" s="17"/>
       <c r="D58" s="21" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E58" s="21" t="s">
         <v>23</v>
@@ -3725,14 +3729,14 @@
     </row>
     <row r="59" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C59" s="17"/>
       <c r="D59" s="21" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E59" s="21" t="s">
         <v>24</v>
@@ -3747,17 +3751,17 @@
     </row>
     <row r="60" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C60" s="17"/>
       <c r="D60" s="21" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E60" s="21" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="F60" s="21"/>
       <c r="G60" s="21"/>
@@ -3768,207 +3772,215 @@
       <c r="L60" s="16"/>
     </row>
     <row r="61" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B61" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C61" s="17"/>
-      <c r="D61" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="E61" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="F61" s="21"/>
-      <c r="G61" s="21"/>
-      <c r="H61" s="20"/>
-      <c r="I61" s="20"/>
+      <c r="A61" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B61" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="C61" s="35"/>
+      <c r="D61" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="E61" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="F61" s="48"/>
+      <c r="G61" s="48"/>
+      <c r="H61" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="I61" s="35" t="s">
+        <v>20</v>
+      </c>
       <c r="J61" s="17"/>
       <c r="K61" s="16"/>
       <c r="L61" s="16"/>
     </row>
     <row r="62" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C62" s="17"/>
-      <c r="D62" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="E62" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="F62" s="21"/>
-      <c r="G62" s="21"/>
-      <c r="H62" s="20"/>
-      <c r="I62" s="20"/>
-      <c r="J62" s="17"/>
+      <c r="D62" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="E62" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F62" s="26"/>
+      <c r="G62" s="26"/>
+      <c r="H62" s="16"/>
+      <c r="I62" s="16"/>
+      <c r="J62" s="16"/>
       <c r="K62" s="16"/>
       <c r="L62" s="16"/>
     </row>
     <row r="63" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="B63" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="C63" s="35"/>
-      <c r="D63" s="33" t="s">
-        <v>60</v>
-      </c>
-      <c r="E63" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="F63" s="48"/>
-      <c r="G63" s="48"/>
-      <c r="H63" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="I63" s="35" t="s">
-        <v>20</v>
-      </c>
+      <c r="A63" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C63" s="17"/>
+      <c r="D63" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="E63" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="F63" s="27"/>
+      <c r="G63" s="27"/>
+      <c r="H63" s="17"/>
+      <c r="I63" s="17"/>
       <c r="J63" s="17"/>
       <c r="K63" s="16"/>
       <c r="L63" s="16"/>
     </row>
     <row r="64" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B64" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C64" s="17"/>
+      <c r="D64" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C64" s="17"/>
-      <c r="D64" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="E64" s="26" t="s">
+      <c r="E64" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F64" s="26"/>
-      <c r="G64" s="26"/>
-      <c r="H64" s="16"/>
-      <c r="I64" s="16"/>
-      <c r="J64" s="16"/>
+      <c r="F64" s="9"/>
+      <c r="G64" s="9"/>
+      <c r="H64" s="8"/>
+      <c r="I64" s="8"/>
+      <c r="J64" s="17"/>
       <c r="K64" s="16"/>
       <c r="L64" s="16"/>
     </row>
     <row r="65" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B65" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C65" s="16"/>
+      <c r="D65" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C65" s="17"/>
-      <c r="D65" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="E65" s="26" t="s">
+      <c r="E65" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F65" s="27"/>
-      <c r="G65" s="27"/>
-      <c r="H65" s="17"/>
-      <c r="I65" s="17"/>
+      <c r="F65" s="9"/>
+      <c r="G65" s="9"/>
+      <c r="H65" s="8"/>
+      <c r="I65" s="8"/>
       <c r="J65" s="17"/>
       <c r="K65" s="16"/>
       <c r="L65" s="16"/>
     </row>
     <row r="66" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B66" s="8" t="s">
+      <c r="A66" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B66" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="C66" s="35"/>
+      <c r="D66" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="C66" s="17"/>
-      <c r="D66" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="E66" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F66" s="9"/>
-      <c r="G66" s="9"/>
-      <c r="H66" s="8"/>
-      <c r="I66" s="8"/>
+      <c r="E66" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="F66" s="39"/>
+      <c r="G66" s="39"/>
+      <c r="H66" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="I66" s="39" t="s">
+        <v>20</v>
+      </c>
       <c r="J66" s="17"/>
       <c r="K66" s="16"/>
       <c r="L66" s="16"/>
     </row>
     <row r="67" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C67" s="16"/>
-      <c r="D67" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="E67" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F67" s="9"/>
-      <c r="G67" s="9"/>
-      <c r="H67" s="8"/>
-      <c r="I67" s="8"/>
-      <c r="J67" s="17"/>
+      <c r="D67" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="E67" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F67" s="26"/>
+      <c r="G67" s="26"/>
+      <c r="H67" s="16"/>
+      <c r="I67" s="16"/>
+      <c r="J67" s="16"/>
       <c r="K67" s="16"/>
       <c r="L67" s="16"/>
+      <c r="M67" s="16"/>
+      <c r="N67" s="16"/>
+      <c r="O67" s="16"/>
+      <c r="P67" s="16"/>
     </row>
     <row r="68" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="B68" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="C68" s="35"/>
-      <c r="D68" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="E68" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="F68" s="39"/>
-      <c r="G68" s="39"/>
-      <c r="H68" s="40" t="s">
-        <v>63</v>
-      </c>
-      <c r="I68" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="J68" s="17"/>
+      <c r="A68" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C68" s="16"/>
+      <c r="D68" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="E68" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="F68" s="26"/>
+      <c r="G68" s="26"/>
+      <c r="H68" s="16"/>
+      <c r="I68" s="16"/>
+      <c r="J68" s="16"/>
       <c r="K68" s="16"/>
       <c r="L68" s="16"/>
+      <c r="M68" s="16"/>
+      <c r="N68" s="16"/>
+      <c r="O68" s="16"/>
+      <c r="P68" s="16"/>
     </row>
     <row r="69" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C69" s="16"/>
-      <c r="D69" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="E69" s="26" t="s">
+      <c r="D69" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E69" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F69" s="26"/>
-      <c r="G69" s="26"/>
-      <c r="H69" s="16"/>
-      <c r="I69" s="16"/>
+      <c r="F69" s="9"/>
+      <c r="G69" s="9"/>
+      <c r="H69" s="8"/>
+      <c r="I69" s="8"/>
       <c r="J69" s="16"/>
       <c r="K69" s="16"/>
       <c r="L69" s="16"/>
@@ -3978,23 +3990,27 @@
       <c r="P69" s="16"/>
     </row>
     <row r="70" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B70" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C70" s="16"/>
-      <c r="D70" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="E70" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="F70" s="26"/>
-      <c r="G70" s="26"/>
-      <c r="H70" s="16"/>
-      <c r="I70" s="16"/>
+      <c r="A70" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B70" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="C70" s="34"/>
+      <c r="D70" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="E70" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="F70" s="40"/>
+      <c r="G70" s="40"/>
+      <c r="H70" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="I70" s="40" t="s">
+        <v>20</v>
+      </c>
       <c r="J70" s="16"/>
       <c r="K70" s="16"/>
       <c r="L70" s="16"/>
@@ -4004,23 +4020,27 @@
       <c r="P70" s="16"/>
     </row>
     <row r="71" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B71" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C71" s="16"/>
-      <c r="D71" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="E71" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="F71" s="26"/>
-      <c r="G71" s="26"/>
-      <c r="H71" s="16"/>
-      <c r="I71" s="16"/>
+      <c r="A71" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B71" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="C71" s="34"/>
+      <c r="D71" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="E71" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="F71" s="40"/>
+      <c r="G71" s="40"/>
+      <c r="H71" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="I71" s="40" t="s">
+        <v>20</v>
+      </c>
       <c r="J71" s="16"/>
       <c r="K71" s="16"/>
       <c r="L71" s="16"/>
@@ -4031,22 +4051,22 @@
     </row>
     <row r="72" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C72" s="16"/>
-      <c r="D72" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E72" s="9" t="s">
+      <c r="D72" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="E72" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="F72" s="9"/>
-      <c r="G72" s="9"/>
-      <c r="H72" s="8"/>
-      <c r="I72" s="8"/>
+      <c r="F72" s="26"/>
+      <c r="G72" s="26"/>
+      <c r="H72" s="16"/>
+      <c r="I72" s="16"/>
       <c r="J72" s="16"/>
       <c r="K72" s="16"/>
       <c r="L72" s="16"/>
@@ -4055,26 +4075,26 @@
       <c r="O72" s="16"/>
       <c r="P72" s="16"/>
     </row>
-    <row r="73" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="B73" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="C73" s="34"/>
-      <c r="D73" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="E73" s="39" t="s">
+    <row r="73" spans="1:16" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B73" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="C73" s="23"/>
+      <c r="D73" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="E73" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="F73" s="40"/>
-      <c r="G73" s="40"/>
-      <c r="H73" s="40" t="s">
-        <v>65</v>
-      </c>
-      <c r="I73" s="40" t="s">
+      <c r="F73" s="25"/>
+      <c r="G73" s="25"/>
+      <c r="H73" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="I73" s="23" t="s">
         <v>20</v>
       </c>
       <c r="J73" s="16"/>
@@ -4087,24 +4107,24 @@
     </row>
     <row r="74" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B74" s="40" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C74" s="34"/>
-      <c r="D74" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="E74" s="39" t="s">
+      <c r="D74" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="E74" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="F74" s="40"/>
-      <c r="G74" s="40"/>
-      <c r="H74" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="I74" s="40" t="s">
+      <c r="F74" s="32"/>
+      <c r="G74" s="32"/>
+      <c r="H74" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="I74" s="34" t="s">
         <v>20</v>
       </c>
       <c r="J74" s="16"/>
@@ -4116,23 +4136,27 @@
       <c r="P74" s="16"/>
     </row>
     <row r="75" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B75" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C75" s="16"/>
-      <c r="D75" s="26" t="s">
+      <c r="A75" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B75" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="C75" s="34"/>
+      <c r="D75" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="E75" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="F75" s="26"/>
-      <c r="G75" s="26"/>
-      <c r="H75" s="16"/>
-      <c r="I75" s="16"/>
+      <c r="E75" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="F75" s="32"/>
+      <c r="G75" s="32"/>
+      <c r="H75" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="I75" s="34" t="s">
+        <v>20</v>
+      </c>
       <c r="J75" s="16"/>
       <c r="K75" s="16"/>
       <c r="L75" s="16"/>
@@ -4141,26 +4165,26 @@
       <c r="O75" s="16"/>
       <c r="P75" s="16"/>
     </row>
-    <row r="76" spans="1:16" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="B76" s="47" t="s">
-        <v>56</v>
-      </c>
-      <c r="C76" s="23"/>
-      <c r="D76" s="25" t="s">
+    <row r="76" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B76" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="C76" s="34"/>
+      <c r="D76" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="E76" s="25" t="s">
+      <c r="E76" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="F76" s="25"/>
-      <c r="G76" s="25"/>
-      <c r="H76" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="I76" s="23" t="s">
+      <c r="F76" s="32"/>
+      <c r="G76" s="32"/>
+      <c r="H76" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="I76" s="34" t="s">
         <v>20</v>
       </c>
       <c r="J76" s="16"/>
@@ -4172,25 +4196,25 @@
       <c r="P76" s="16"/>
     </row>
     <row r="77" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="B77" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="C77" s="34"/>
-      <c r="D77" s="32" t="s">
+      <c r="A77" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B77" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="C77" s="23"/>
+      <c r="D77" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="E77" s="32" t="s">
+      <c r="E77" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="F77" s="32"/>
-      <c r="G77" s="32"/>
-      <c r="H77" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="I77" s="34" t="s">
+      <c r="F77" s="25"/>
+      <c r="G77" s="25"/>
+      <c r="H77" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="I77" s="23" t="s">
         <v>20</v>
       </c>
       <c r="J77" s="16"/>
@@ -4202,143 +4226,53 @@
       <c r="P77" s="16"/>
     </row>
     <row r="78" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="B78" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="C78" s="34"/>
-      <c r="D78" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="E78" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="F78" s="32"/>
-      <c r="G78" s="32"/>
-      <c r="H78" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="I78" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="J78" s="16"/>
-      <c r="K78" s="16"/>
-      <c r="L78" s="16"/>
-      <c r="M78" s="16"/>
-      <c r="N78" s="16"/>
-      <c r="O78" s="16"/>
-      <c r="P78" s="16"/>
+      <c r="A78" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C78" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D78" s="8"/>
+      <c r="E78" s="8"/>
+      <c r="F78" s="8"/>
+      <c r="G78" s="8"/>
+      <c r="H78" s="8"/>
+      <c r="I78" s="8"/>
     </row>
     <row r="79" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="30" t="s">
-        <v>34</v>
+      <c r="A79" s="47" t="s">
+        <v>33</v>
       </c>
       <c r="B79" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="C79" s="34"/>
-      <c r="D79" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="E79" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="F79" s="32"/>
-      <c r="G79" s="32"/>
-      <c r="H79" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="I79" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="J79" s="16"/>
-      <c r="K79" s="16"/>
-      <c r="L79" s="16"/>
-      <c r="M79" s="16"/>
-      <c r="N79" s="16"/>
-      <c r="O79" s="16"/>
-      <c r="P79" s="16"/>
+      <c r="C79" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="D79" s="40"/>
+      <c r="E79" s="40"/>
+      <c r="F79" s="40"/>
+      <c r="G79" s="40"/>
+      <c r="H79" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="I79" s="40" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="80" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="B80" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="C80" s="34"/>
-      <c r="D80" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="E80" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="F80" s="32"/>
-      <c r="G80" s="32"/>
-      <c r="H80" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="I80" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="J80" s="16"/>
-      <c r="K80" s="16"/>
-      <c r="L80" s="16"/>
-      <c r="M80" s="16"/>
-      <c r="N80" s="16"/>
-      <c r="O80" s="16"/>
-      <c r="P80" s="16"/>
-    </row>
-    <row r="81" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B81" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C81" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D81" s="8"/>
-      <c r="E81" s="8"/>
-      <c r="F81" s="8"/>
-      <c r="G81" s="8"/>
-      <c r="H81" s="8"/>
-      <c r="I81" s="8"/>
-    </row>
-    <row r="82" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="B82" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="C82" s="47" t="s">
-        <v>31</v>
-      </c>
-      <c r="D82" s="47"/>
-      <c r="E82" s="47"/>
-      <c r="F82" s="47"/>
-      <c r="G82" s="47"/>
-      <c r="H82" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="I82" s="47" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="8"/>
-      <c r="C83" s="8"/>
-      <c r="D83" s="9"/>
-      <c r="E83" s="9"/>
-      <c r="F83" s="9"/>
-      <c r="G83" s="9"/>
+      <c r="B80" s="8"/>
+      <c r="C80" s="8"/>
+      <c r="D80" s="9"/>
+      <c r="E80" s="9"/>
+      <c r="F80" s="9"/>
+      <c r="G80" s="9"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I82"/>
+  <autoFilter ref="A1:I79"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>

</xml_diff>